<commit_message>
Deploying to gh-pages from @ EDGEResearch-CA/TMAtools@76285158a10b06eb913fa03ef737ac0f0b690ee2 🚀
</commit_message>
<xml_diff>
--- a/reference/deconvoluted_tma.xlsx
+++ b/reference/deconvoluted_tma.xlsx
@@ -365,17 +365,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>er.c1</t>
+          <t>ER.c1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>er.c2</t>
+          <t>ER.c2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>er.c3</t>
+          <t>ER.c3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">

</xml_diff>